<commit_message>
update corrected system adresses
</commit_message>
<xml_diff>
--- a/docs/Disk Map CPM-65 JC II.xlsx
+++ b/docs/Disk Map CPM-65 JC II.xlsx
@@ -60,15 +60,6 @@
     <t>0 .. 31</t>
   </si>
   <si>
-    <t>$B000 .. $B7FF</t>
-  </si>
-  <si>
-    <t>$AC00 .. $AFFF</t>
-  </si>
-  <si>
-    <t>$B800 .. $BFFF</t>
-  </si>
-  <si>
     <t>CPM-65 JC II Version</t>
   </si>
   <si>
@@ -163,6 +154,15 @@
   </si>
   <si>
     <t>DISKDEFS</t>
+  </si>
+  <si>
+    <t>$CC00 .. $CFFF</t>
+  </si>
+  <si>
+    <t>$D000 .. $D7FF</t>
+  </si>
+  <si>
+    <t>$D800 .. $DFFF</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -629,7 +629,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.45">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -681,43 +681,43 @@
     <row r="8" spans="1:4">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="10"/>
       <c r="B9" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>13</v>
@@ -762,12 +762,12 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="13">
         <v>7</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="13">
         <v>3</v>
@@ -785,18 +785,18 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="13">
         <v>32</v>
@@ -805,25 +805,25 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="13">
         <v>32</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" s="13">
         <v>32</v>
@@ -846,22 +846,22 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>256</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>128</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>32</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>2048</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>128</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -917,15 +917,15 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>